<commit_message>
add the profile functionality
</commit_message>
<xml_diff>
--- a/server/excel/kamdilichukwu2020@gmail.comKamdilichukwuOkolo.xlsx
+++ b/server/excel/kamdilichukwu2020@gmail.comKamdilichukwuOkolo.xlsx
@@ -455,7 +455,7 @@
         <v>Address</v>
       </c>
       <c r="B7" t="str">
-        <v xml:space="preserve">29 mbaukwu street </v>
+        <v xml:space="preserve">28 mbaukwu street </v>
       </c>
     </row>
     <row r="8">
@@ -463,7 +463,7 @@
         <v>Account Number</v>
       </c>
       <c r="B8" t="str">
-        <v>003831123</v>
+        <v>2211433744</v>
       </c>
     </row>
     <row r="9">

</xml_diff>